<commit_message>
add requirements.txt and test api call
</commit_message>
<xml_diff>
--- a/Unprocessed Files/Lines.xlsx
+++ b/Unprocessed Files/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adko8\OneDrive\Desktop\TARS\Unprocessed Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BC1903B-459B-41C3-B282-7B999DABB8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B2DEA3-F84A-43C5-A34A-0BAFA12788F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{411462C6-0553-4045-81F6-2A96E886D10C}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t>Text</t>
   </si>
   <si>
-    <t>Voice</t>
-  </si>
-  <si>
     <t>May the Force be with you.</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>I'll be back.</t>
+  </si>
+  <si>
+    <t>Voice ID</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,7 +447,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -455,10 +455,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -466,10 +466,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add function to save voices to excel file
</commit_message>
<xml_diff>
--- a/Unprocessed Files/Lines.xlsx
+++ b/Unprocessed Files/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adko8\OneDrive\Desktop\TARS\Unprocessed Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B2DEA3-F84A-43C5-A34A-0BAFA12788F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DFC359-2E05-4A91-9C31-70C7CC719D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{411462C6-0553-4045-81F6-2A96E886D10C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Line ID</t>
   </si>
@@ -47,16 +47,25 @@
     <t>May the Force be with you.</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>I'll be back.</t>
   </si>
   <si>
     <t>Voice ID</t>
+  </si>
+  <si>
+    <t>Voice Name</t>
+  </si>
+  <si>
+    <t>t0jbNlBVZ17f02VDIeMI</t>
+  </si>
+  <si>
+    <t>Jessie</t>
+  </si>
+  <si>
+    <t>zcAOhNBS3c14rBihAFp1</t>
+  </si>
+  <si>
+    <t>Giovanni</t>
   </si>
 </sst>
 </file>
@@ -428,18 +437,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE0B8FF-D7DA-43E3-8589-72A8DE89571B}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,10 +457,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -458,18 +471,24 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>